<commit_message>
change generic user import service and command to specific import employer service and command
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -40,19 +40,19 @@
     <t xml:space="preserve">city</t>
   </si>
   <si>
-    <t xml:space="preserve">degiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info@degiro.nl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeGiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amstelplein 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1096HA</t>
+    <t xml:space="preserve">hyves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@hyves.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisweg 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1043AP</t>
   </si>
   <si>
     <t xml:space="preserve">Amsterdam</t>
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -85,12 +85,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -137,16 +131,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -170,13 +160,13 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.43"/>
   </cols>
@@ -225,7 +215,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -299,7 +289,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="info@degiro.nl"/>
+    <hyperlink ref="B2" r:id="rId1" display="info@hyves.nl"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>